<commit_message>
funktion von load_page in procedures.php
</commit_message>
<xml_diff>
--- a/Sonstiges/TODO.xlsx
+++ b/Sonstiges/TODO.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t>Aufgabe</t>
   </si>
@@ -99,13 +99,19 @@
   </si>
   <si>
     <t>Abstimmung: zweiter Selector nur anzeigen wenns sinn macht</t>
+  </si>
+  <si>
+    <t>Gruppe löschen -&gt; anlegen Fehler?</t>
+  </si>
+  <si>
+    <t>ü</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,6 +126,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Wingdings"/>
+      <charset val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -142,7 +154,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -158,6 +170,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -438,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F16"/>
+  <dimension ref="A2:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -540,6 +553,7 @@
         <v>15</v>
       </c>
       <c r="D8" s="3"/>
+      <c r="E8" s="7"/>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
@@ -595,7 +609,10 @@
         <v>22</v>
       </c>
       <c r="C14" t="s">
-        <v>14</v>
+        <v>3</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -619,6 +636,20 @@
       <c r="C16" t="s">
         <v>14</v>
       </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>15</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>